<commit_message>
Updating units for external data (mks)
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="15315" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="15315" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Cost" sheetId="1" r:id="rId1"/>
     <sheet name="GHG" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>Diameter</t>
   </si>
@@ -139,13 +139,25 @@
   </si>
   <si>
     <t>(kg-CO2-e/ft/yr)</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>kg-CO2-e/m/s</t>
+  </si>
+  <si>
+    <t>KMS units</t>
+  </si>
+  <si>
+    <t>$/m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,18 +215,34 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -225,6 +253,7 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
@@ -314,16 +343,25 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="49452928"/>
-        <c:axId val="49454464"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="134726016"/>
+        <c:axId val="134727936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49452928"/>
+        <c:axId val="134726016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -342,19 +380,22 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49454464"/>
+        <c:crossAx val="134727936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49454464"/>
+        <c:axId val="134727936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -374,20 +415,24 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49452928"/>
+        <c:crossAx val="134726016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -395,12 +440,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -717,6 +774,8 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -808,9 +867,13 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:trendline>
             <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -850,31 +913,45 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="44847104"/>
-        <c:axId val="44848640"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="134651264"/>
+        <c:axId val="134657152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44847104"/>
+        <c:axId val="134651264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44848640"/>
+        <c:crossAx val="134657152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44848640"/>
+        <c:axId val="134657152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44847104"/>
+        <c:crossAx val="134651264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -882,12 +959,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -895,13 +975,24 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -912,12 +1003,13 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15722116519821638"/>
-                  <c:y val="-6.640944881889764E-2"/>
+                  <c:x val="-0.15722116519821641"/>
+                  <c:y val="-6.6409448818897654E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1001,16 +1093,25 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="45078400"/>
-        <c:axId val="45076480"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="143017472"/>
+        <c:axId val="143019392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45078400"/>
+        <c:axId val="143017472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1029,19 +1130,22 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45076480"/>
+        <c:crossAx val="143019392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45076480"/>
+        <c:axId val="143019392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1061,16 +1165,198 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45078400"/>
+        <c:crossAx val="143017472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Cost!$L$5:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.254</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.50800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.71099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.76200000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Cost!$M$5:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>8.31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.66</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.69</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="49184768"/>
+        <c:axId val="49178880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="49184768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49178880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="49178880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49184768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1144,16 +1430,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1167,6 +1453,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1250,6 +1566,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1284,6 +1601,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1459,14 +1777,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
@@ -1474,21 +1792,25 @@
     <col min="7" max="7" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1">
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="L2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1521,8 +1843,14 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>102</v>
       </c>
@@ -1545,8 +1873,23 @@
         <v>2.5335365853658538</v>
       </c>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="L5">
+        <f>A5/1000</f>
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="M5">
+        <f>B5</f>
+        <v>8.31</v>
+      </c>
+      <c r="O5">
+        <v>0.11</v>
+      </c>
+      <c r="P5">
+        <f>VLOOKUP(O5,L5:M16,2)</f>
+        <v>8.31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>152</v>
       </c>
@@ -1569,8 +1912,16 @@
         <v>3.0792682926829271</v>
       </c>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="L6">
+        <f t="shared" ref="L6:L16" si="3">A6/1000</f>
+        <v>0.152</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M16" si="4">B6</f>
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>203</v>
       </c>
@@ -1593,8 +1944,16 @@
         <v>3.6890243902439024</v>
       </c>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>254</v>
       </c>
@@ -1617,8 +1976,16 @@
         <v>3.9512195121951224</v>
       </c>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>0.254</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>12.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>305</v>
       </c>
@@ -1641,8 +2008,16 @@
         <v>4.6402439024390247</v>
       </c>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>15.22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>356</v>
       </c>
@@ -1665,8 +2040,16 @@
         <v>5.0670731707317076</v>
       </c>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>16.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>406</v>
       </c>
@@ -1689,8 +2072,16 @@
         <v>5.9176829268292686</v>
       </c>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>19.41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>457</v>
       </c>
@@ -1713,8 +2104,16 @@
         <v>6.7682926829268295</v>
       </c>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>508</v>
       </c>
@@ -1737,8 +2136,16 @@
         <v>7.5182926829268295</v>
       </c>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>24.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>610</v>
       </c>
@@ -1761,8 +2168,16 @@
         <v>10.88109756097561</v>
       </c>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>0.61</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>35.69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>711</v>
       </c>
@@ -1785,8 +2200,16 @@
         <v>12.219512195121952</v>
       </c>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>40.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>762</v>
       </c>
@@ -1809,14 +2232,23 @@
         <v>12.987804878048781</v>
       </c>
       <c r="I16" s="1"/>
-    </row>
-    <row r="20" spans="1:8" s="3" customFormat="1">
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1830,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1844,7 +2276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>500</v>
       </c>
@@ -1859,8 +2291,16 @@
         <f>B23*1000</f>
         <v>14020</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="L23">
+        <f>A23</f>
+        <v>500</v>
+      </c>
+      <c r="M23">
+        <f>H23</f>
+        <v>14020</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1000</v>
       </c>
@@ -1868,15 +2308,23 @@
         <v>30.64</v>
       </c>
       <c r="G24" s="6">
-        <f t="shared" ref="G24:G28" si="3">A24*35.3146667</f>
+        <f t="shared" ref="G24:G28" si="5">A24*35.3146667</f>
         <v>35314.666699999994</v>
       </c>
       <c r="H24">
-        <f t="shared" ref="H24:H28" si="4">B24*1000</f>
+        <f t="shared" ref="H24:H28" si="6">B24*1000</f>
         <v>30640</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="L24">
+        <f t="shared" ref="L24:L28" si="7">A24</f>
+        <v>1000</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M28" si="8">H24</f>
+        <v>30640</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2000</v>
       </c>
@@ -1884,15 +2332,23 @@
         <v>61.21</v>
       </c>
       <c r="G25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>70629.333399999989</v>
       </c>
       <c r="H25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>61210</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="L25">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="8"/>
+        <v>61210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3750</v>
       </c>
@@ -1900,15 +2356,23 @@
         <v>87.46</v>
       </c>
       <c r="G26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>132430.00012499999</v>
       </c>
       <c r="H26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>87460</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="L26">
+        <f t="shared" si="7"/>
+        <v>3750</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="8"/>
+        <v>87460</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5000</v>
       </c>
@@ -1916,15 +2380,23 @@
         <v>122.42</v>
       </c>
       <c r="G27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>176573.33349999998</v>
       </c>
       <c r="H27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>122420</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="L27">
+        <f t="shared" si="7"/>
+        <v>5000</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="8"/>
+        <v>122420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10000</v>
       </c>
@@ -1932,21 +2404,30 @@
         <v>174.93</v>
       </c>
       <c r="G28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>353146.66699999996</v>
       </c>
       <c r="H28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>174930</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" s="3" customFormat="1">
+      <c r="L28">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="8"/>
+        <v>174930</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="L30"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1974,7 +2455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>102</v>
       </c>
@@ -1993,8 +2474,16 @@
         <f>B33</f>
         <v>323</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="L33">
+        <f>A33/1000</f>
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="M33">
+        <f>B33</f>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>152</v>
       </c>
@@ -2002,19 +2491,27 @@
         <v>529</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E44" si="5">A34/10/2.54</f>
+        <f t="shared" ref="E34:E44" si="9">A34/10/2.54</f>
         <v>5.984251968503937</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" ref="G34" si="6">ROUND(E34,0)</f>
+        <f t="shared" ref="G34" si="10">ROUND(E34,0)</f>
         <v>6</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H44" si="7">B34</f>
+        <f t="shared" ref="H34:H44" si="11">B34</f>
         <v>529</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="L34">
+        <f t="shared" ref="L34:L44" si="12">A34/1000</f>
+        <v>0.152</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ref="M34:M44" si="13">B34</f>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>203</v>
       </c>
@@ -2022,19 +2519,27 @@
         <v>779</v>
       </c>
       <c r="E35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7.9921259842519685</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" ref="G35" si="8">ROUND(E35,0)</f>
+        <f t="shared" ref="G35" si="14">ROUND(E35,0)</f>
         <v>8</v>
       </c>
       <c r="H35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>779</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="L35">
+        <f t="shared" si="12"/>
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="13"/>
+        <v>779</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>254</v>
       </c>
@@ -2042,19 +2547,27 @@
         <v>1113</v>
       </c>
       <c r="E36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" ref="G36" si="9">ROUND(E36,0)</f>
+        <f t="shared" ref="G36" si="15">ROUND(E36,0)</f>
         <v>10</v>
       </c>
       <c r="H36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1113</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="L36">
+        <f t="shared" si="12"/>
+        <v>0.254</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="13"/>
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>305</v>
       </c>
@@ -2062,19 +2575,27 @@
         <v>1892</v>
       </c>
       <c r="E37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12.007874015748031</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" ref="G37" si="10">ROUND(E37,0)</f>
+        <f t="shared" ref="G37" si="16">ROUND(E37,0)</f>
         <v>12</v>
       </c>
       <c r="H37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1892</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="L37">
+        <f t="shared" si="12"/>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="13"/>
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>356</v>
       </c>
@@ -2082,19 +2603,27 @@
         <v>2282</v>
       </c>
       <c r="E38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14.015748031496063</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" ref="G38" si="11">ROUND(E38,0)</f>
+        <f t="shared" ref="G38" si="17">ROUND(E38,0)</f>
         <v>14</v>
       </c>
       <c r="H38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>2282</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="L38">
+        <f t="shared" si="12"/>
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="13"/>
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>406</v>
       </c>
@@ -2102,19 +2631,27 @@
         <v>4063</v>
       </c>
       <c r="E39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15.984251968503937</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" ref="G39" si="12">ROUND(E39,0)</f>
+        <f t="shared" ref="G39" si="18">ROUND(E39,0)</f>
         <v>16</v>
       </c>
       <c r="H39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4063</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="L39">
+        <f t="shared" si="12"/>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="13"/>
+        <v>4063</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>457</v>
       </c>
@@ -2122,19 +2659,27 @@
         <v>4452</v>
       </c>
       <c r="E40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>17.99212598425197</v>
       </c>
       <c r="G40" s="2">
-        <f t="shared" ref="G40" si="13">ROUND(E40,0)</f>
+        <f t="shared" ref="G40" si="19">ROUND(E40,0)</f>
         <v>18</v>
       </c>
       <c r="H40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4452</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="L40">
+        <f t="shared" si="12"/>
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="13"/>
+        <v>4452</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>508</v>
       </c>
@@ -2142,19 +2687,27 @@
         <v>4564</v>
       </c>
       <c r="E41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="G41" s="2">
-        <f t="shared" ref="G41" si="14">ROUND(E41,0)</f>
+        <f t="shared" ref="G41" si="20">ROUND(E41,0)</f>
         <v>20</v>
       </c>
       <c r="H41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4564</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="L41">
+        <f t="shared" si="12"/>
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="13"/>
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>610</v>
       </c>
@@ -2162,19 +2715,27 @@
         <v>5287</v>
       </c>
       <c r="E42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>24.015748031496063</v>
       </c>
       <c r="G42" s="2">
-        <f t="shared" ref="G42" si="15">ROUND(E42,0)</f>
+        <f t="shared" ref="G42" si="21">ROUND(E42,0)</f>
         <v>24</v>
       </c>
       <c r="H42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5287</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="L42">
+        <f t="shared" si="12"/>
+        <v>0.61</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="13"/>
+        <v>5287</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>711</v>
       </c>
@@ -2182,19 +2743,27 @@
         <v>6122</v>
       </c>
       <c r="E43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>27.992125984251967</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" ref="G43" si="16">ROUND(E43,0)</f>
+        <f t="shared" ref="G43" si="22">ROUND(E43,0)</f>
         <v>28</v>
       </c>
       <c r="H43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6122</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="L43">
+        <f t="shared" si="12"/>
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="13"/>
+        <v>6122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>762</v>
       </c>
@@ -2202,19 +2771,27 @@
         <v>6790</v>
       </c>
       <c r="E44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="G44" s="2">
-        <f t="shared" ref="G44" si="17">ROUND(E44,0)</f>
+        <f t="shared" ref="G44" si="23">ROUND(E44,0)</f>
         <v>30</v>
       </c>
       <c r="H44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6790</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="L44">
+        <f>A44/1000</f>
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="13"/>
+        <v>6790</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -2231,7 +2808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2246,7 +2823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>8</v>
       </c>
@@ -2266,7 +2843,7 @@
         <v>4133</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>9</v>
       </c>
@@ -2286,7 +2863,7 @@
         <v>3563</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>10</v>
       </c>
@@ -2306,7 +2883,7 @@
         <v>4339</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>11</v>
       </c>
@@ -2326,7 +2903,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2346,7 +2923,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -2366,7 +2943,7 @@
         <v>3307</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -2383,7 +2960,7 @@
         <v>2850</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -2400,7 +2977,7 @@
         <v>4554</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -2417,7 +2994,7 @@
         <v>3820</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -2434,7 +3011,7 @@
         <v>4823</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>0.1</v>
       </c>
@@ -2445,7 +3022,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -2456,7 +3033,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>8</v>
       </c>
@@ -2467,7 +3044,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>8</v>
       </c>
@@ -2482,7 +3059,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>8</v>
       </c>
@@ -2501,7 +3078,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9</v>
       </c>
@@ -2512,7 +3089,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9</v>
       </c>
@@ -2527,7 +3104,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9</v>
       </c>
@@ -2546,7 +3123,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>10</v>
       </c>
@@ -2557,7 +3134,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>10</v>
       </c>
@@ -2572,7 +3149,7 @@
         <v>3450</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>10</v>
       </c>
@@ -2591,7 +3168,7 @@
         <v>6250</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>11</v>
       </c>
@@ -2602,7 +3179,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>11</v>
       </c>
@@ -2617,7 +3194,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>11</v>
       </c>
@@ -2636,7 +3213,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -2647,7 +3224,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -2662,7 +3239,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -2681,7 +3258,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>13</v>
       </c>
@@ -2692,7 +3269,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -2707,7 +3284,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>13</v>
       </c>
@@ -2726,7 +3303,7 @@
         <v>3125</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -2737,7 +3314,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -2752,7 +3329,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -2771,7 +3348,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -2782,7 +3359,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>15</v>
       </c>
@@ -2797,7 +3374,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>15</v>
       </c>
@@ -2816,7 +3393,7 @@
         <v>6240</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -2827,7 +3404,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -2842,7 +3419,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -2861,7 +3438,7 @@
         <v>4080</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>17</v>
       </c>
@@ -2872,7 +3449,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>17</v>
       </c>
@@ -2887,7 +3464,7 @@
         <v>4140</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>17</v>
       </c>
@@ -2914,14 +3491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -2929,17 +3506,21 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -2951,7 +3532,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -2965,7 +3546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2978,8 +3559,14 @@
       <c r="H4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>102</v>
       </c>
@@ -2998,8 +3585,16 @@
         <f>B5/3.28</f>
         <v>1.7987804878048783</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="L5">
+        <f>A5/1000</f>
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="M5">
+        <f>B5</f>
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>152</v>
       </c>
@@ -3018,8 +3613,16 @@
         <f t="shared" ref="H6:H16" si="1">B6/3.28</f>
         <v>2.9603658536585371</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="L6">
+        <f t="shared" ref="L6:L16" si="2">A6/1000</f>
+        <v>0.152</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M16" si="3">B6</f>
+        <v>9.7100000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>203</v>
       </c>
@@ -3031,15 +3634,23 @@
         <v>7.9921259842519685</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ref="G5:G16" si="2">ROUND(E7,0)</f>
+        <f t="shared" ref="G7:G15" si="4">ROUND(E7,0)</f>
         <v>8</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>13.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>254</v>
       </c>
@@ -3051,15 +3662,23 @@
         <v>10</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
         <v>5.6189024390243905</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>0.254</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>18.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>305</v>
       </c>
@@ -3071,15 +3690,23 @@
         <v>12.007874015748031</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="1"/>
         <v>7.0609756097560981</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>23.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>356</v>
       </c>
@@ -3091,15 +3718,23 @@
         <v>14.015748031496063</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
         <v>8.5640243902439028</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>28.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>406</v>
       </c>
@@ -3111,15 +3746,23 @@
         <v>15.984251968503937</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
         <v>10.088414634146343</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>33.090000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>457</v>
       </c>
@@ -3131,15 +3774,23 @@
         <v>17.99212598425197</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
         <v>11.692073170731708</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>38.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>508</v>
       </c>
@@ -3151,15 +3802,23 @@
         <v>20</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
         <v>13.341463414634147</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>43.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>610</v>
       </c>
@@ -3171,15 +3830,23 @@
         <v>24.015748031496063</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
         <v>16.765243902439025</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>0.61</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>54.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>711</v>
       </c>
@@ -3191,15 +3858,23 @@
         <v>27.992125984251967</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
         <v>20.295731707317071</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>66.569999999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>762</v>
       </c>
@@ -3218,8 +3893,16 @@
         <f t="shared" si="1"/>
         <v>22.128048780487806</v>
       </c>
-    </row>
-    <row r="33" spans="3:3">
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>72.58</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="5"/>
     </row>
   </sheetData>
@@ -3228,12 +3911,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>